<commit_message>
Sửa phần tìm kiếm
Sửa phần tìm kiếm
Các file:
+ HomeController
+ ListStudent
</commit_message>
<xml_diff>
--- a/Quản lý điểm thi/Excel/Home/mau_xua_excel.xlsx
+++ b/Quản lý điểm thi/Excel/Home/mau_xua_excel.xlsx
@@ -451,13 +451,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="20.44140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" style="3" customWidth="1"/>
@@ -469,7 +469,7 @@
     <col min="11" max="11" width="20.109375" style="3" customWidth="1"/>
     <col min="12" max="12" width="47" style="3" customWidth="1"/>
     <col min="13" max="13" width="47.21875" style="3" customWidth="1"/>
-    <col min="14" max="14" width="9.109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="20.44140625" style="3" customWidth="1"/>
     <col min="15" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>

</xml_diff>